<commit_message>
fixed typo in carbon stock classification key file, further edits to all three tabs. main DISPLAY functionalities present. still need to build out interactive functionalities.
</commit_message>
<xml_diff>
--- a/carbon_stock_cfs/class_descriptions_key.xlsx
+++ b/carbon_stock_cfs/class_descriptions_key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\catli\Documents\ESM 244 Labs\esm244-final-project\carbon_stock_cfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065685B2-C71B-48DD-AA35-AF568219D2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6AFCD7-F2D4-4791-87FD-6E2B238A03B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11724" yWindow="1668" windowWidth="21468" windowHeight="9552" xr2:uid="{45869698-FF38-47F4-AB33-F6790227560A}"/>
+    <workbookView xWindow="84" yWindow="4308" windowWidth="21468" windowHeight="9552" xr2:uid="{45869698-FF38-47F4-AB33-F6790227560A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Shrub/Scrub</t>
   </si>
   <si>
-    <t>Glassland/Herbaceous</t>
-  </si>
-  <si>
     <t>Sedge/Herbaceous</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Emergent Herbaceous Wetlands</t>
+  </si>
+  <si>
+    <t>Grassland/Herbaceous</t>
   </si>
 </sst>
 </file>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4B218F-8522-4857-8289-21EDEFE89DE2}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,7 +570,7 @@
         <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -578,7 +578,7 @@
         <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -586,7 +586,7 @@
         <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -602,7 +602,7 @@
         <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -610,7 +610,7 @@
         <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -618,7 +618,7 @@
         <v>90</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
         <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>